<commit_message>
Working on the backend of the project
</commit_message>
<xml_diff>
--- a/docs/blog.csv.xlsx
+++ b/docs/blog.csv.xlsx
@@ -8,17 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alank\source\repos\blog-listing-application\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C27D5BB-7213-4AA8-9FD7-3810DA941C0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{225F052E-6E24-4C1A-A64B-9013EFFF98A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="2340" windowWidth="18000" windowHeight="9360" activeTab="3" xr2:uid="{1DD7D00E-AB4E-489D-B05C-50AAA1CEC988}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{1DD7D00E-AB4E-489D-B05C-50AAA1CEC988}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
     <sheet name="Blogs" sheetId="4" r:id="rId2"/>
     <sheet name="Authors" sheetId="3" r:id="rId3"/>
     <sheet name="Titles" sheetId="7" r:id="rId4"/>
-    <sheet name="Departments" sheetId="5" r:id="rId5"/>
-    <sheet name="Topics" sheetId="2" r:id="rId6"/>
+    <sheet name="Topics" sheetId="2" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="261">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="155">
   <si>
     <t>Id</t>
   </si>
@@ -207,18 +206,6 @@
     <t>Contents</t>
   </si>
   <si>
-    <t>DepartmentId</t>
-  </si>
-  <si>
-    <t>PhoneNumber</t>
-  </si>
-  <si>
-    <t>ChairPerson</t>
-  </si>
-  <si>
-    <t>DepartmentName</t>
-  </si>
-  <si>
     <t>Boatwright</t>
   </si>
   <si>
@@ -354,321 +341,6 @@
     <t>divane@illinois.edu</t>
   </si>
   <si>
-    <t>Seekings</t>
-  </si>
-  <si>
-    <t>Allx</t>
-  </si>
-  <si>
-    <t>aseekingsf@aol.com</t>
-  </si>
-  <si>
-    <t>Rubinowicz</t>
-  </si>
-  <si>
-    <t>Shanta</t>
-  </si>
-  <si>
-    <t>srubinowiczg@stanford.edu</t>
-  </si>
-  <si>
-    <t>Glendza</t>
-  </si>
-  <si>
-    <t>Sloane</t>
-  </si>
-  <si>
-    <t>sglendzah@ibm.com</t>
-  </si>
-  <si>
-    <t>Kilban</t>
-  </si>
-  <si>
-    <t>Wendeline</t>
-  </si>
-  <si>
-    <t>wkilbani@examiner.com</t>
-  </si>
-  <si>
-    <t>Noni</t>
-  </si>
-  <si>
-    <t>Roshelle</t>
-  </si>
-  <si>
-    <t>rnonij@ebay.com</t>
-  </si>
-  <si>
-    <t>Halse</t>
-  </si>
-  <si>
-    <t>Corene</t>
-  </si>
-  <si>
-    <t>chalsek@nps.gov</t>
-  </si>
-  <si>
-    <t>Olcot</t>
-  </si>
-  <si>
-    <t>Katlin</t>
-  </si>
-  <si>
-    <t>kolcotl@free.fr</t>
-  </si>
-  <si>
-    <t>Paike</t>
-  </si>
-  <si>
-    <t>Merla</t>
-  </si>
-  <si>
-    <t>mpaikem@sphinn.com</t>
-  </si>
-  <si>
-    <t>Rolfi</t>
-  </si>
-  <si>
-    <t>Georgetta</t>
-  </si>
-  <si>
-    <t>grolfin@usa.gov</t>
-  </si>
-  <si>
-    <t>MacEvilly</t>
-  </si>
-  <si>
-    <t>Demetre</t>
-  </si>
-  <si>
-    <t>dmacevillyo@upenn.edu</t>
-  </si>
-  <si>
-    <t>Keddie</t>
-  </si>
-  <si>
-    <t>Lissi</t>
-  </si>
-  <si>
-    <t>lkeddiep@tripadvisor.com</t>
-  </si>
-  <si>
-    <t>Scorrer</t>
-  </si>
-  <si>
-    <t>Theresita</t>
-  </si>
-  <si>
-    <t>tscorrerq@intel.com</t>
-  </si>
-  <si>
-    <t>Bilverstone</t>
-  </si>
-  <si>
-    <t>Joell</t>
-  </si>
-  <si>
-    <t>jbilverstoner@lycos.com</t>
-  </si>
-  <si>
-    <t>Bowle</t>
-  </si>
-  <si>
-    <t>Vivienne</t>
-  </si>
-  <si>
-    <t>vbowles@prnewswire.com</t>
-  </si>
-  <si>
-    <t>Stranio</t>
-  </si>
-  <si>
-    <t>Rodi</t>
-  </si>
-  <si>
-    <t>rstraniot@histats.com</t>
-  </si>
-  <si>
-    <t>Domnick</t>
-  </si>
-  <si>
-    <t>Alfonso</t>
-  </si>
-  <si>
-    <t>adomnicku@mysql.com</t>
-  </si>
-  <si>
-    <t>Beneze</t>
-  </si>
-  <si>
-    <t>Kyle</t>
-  </si>
-  <si>
-    <t>kbenezev@cmu.edu</t>
-  </si>
-  <si>
-    <t>Shewen</t>
-  </si>
-  <si>
-    <t>Artie</t>
-  </si>
-  <si>
-    <t>ashewenw@instagram.com</t>
-  </si>
-  <si>
-    <t>Arsmith</t>
-  </si>
-  <si>
-    <t>Ermengarde</t>
-  </si>
-  <si>
-    <t>earsmithx@freewebs.com</t>
-  </si>
-  <si>
-    <t>Rhyme</t>
-  </si>
-  <si>
-    <t>Amber</t>
-  </si>
-  <si>
-    <t>arhymey@themeforest.net</t>
-  </si>
-  <si>
-    <t>Beecham</t>
-  </si>
-  <si>
-    <t>Eydie</t>
-  </si>
-  <si>
-    <t>ebeechamz@creativecommons.org</t>
-  </si>
-  <si>
-    <t>Summerside</t>
-  </si>
-  <si>
-    <t>Kristos</t>
-  </si>
-  <si>
-    <t>ksummerside10@npr.org</t>
-  </si>
-  <si>
-    <t>Linham</t>
-  </si>
-  <si>
-    <t>Celina</t>
-  </si>
-  <si>
-    <t>clinham11@paypal.com</t>
-  </si>
-  <si>
-    <t>O'Rowane</t>
-  </si>
-  <si>
-    <t>Halley</t>
-  </si>
-  <si>
-    <t>horowane12@51.la</t>
-  </si>
-  <si>
-    <t>Cunde</t>
-  </si>
-  <si>
-    <t>Bailey</t>
-  </si>
-  <si>
-    <t>bcunde13@uol.com.br</t>
-  </si>
-  <si>
-    <t>Crehan</t>
-  </si>
-  <si>
-    <t>Thornie</t>
-  </si>
-  <si>
-    <t>tcrehan14@gov.uk</t>
-  </si>
-  <si>
-    <t>Lodeke</t>
-  </si>
-  <si>
-    <t>Jabez</t>
-  </si>
-  <si>
-    <t>jlodeke15@vk.com</t>
-  </si>
-  <si>
-    <t>Banthorpe</t>
-  </si>
-  <si>
-    <t>Calli</t>
-  </si>
-  <si>
-    <t>cbanthorpe16@dagondesign.com</t>
-  </si>
-  <si>
-    <t>Totaro</t>
-  </si>
-  <si>
-    <t>Carri</t>
-  </si>
-  <si>
-    <t>ctotaro17@pbs.org</t>
-  </si>
-  <si>
-    <t>Wessing</t>
-  </si>
-  <si>
-    <t>Astrix</t>
-  </si>
-  <si>
-    <t>awessing18@mysql.com</t>
-  </si>
-  <si>
-    <t>Alessandrelli</t>
-  </si>
-  <si>
-    <t>Nevil</t>
-  </si>
-  <si>
-    <t>nalessandrelli19@technorati.com</t>
-  </si>
-  <si>
-    <t>Purser</t>
-  </si>
-  <si>
-    <t>Zelig</t>
-  </si>
-  <si>
-    <t>zpurser1a@hao123.com</t>
-  </si>
-  <si>
-    <t>McKeighan</t>
-  </si>
-  <si>
-    <t>Kelila</t>
-  </si>
-  <si>
-    <t>kmckeighan1b@bloomberg.com</t>
-  </si>
-  <si>
-    <t>Rivenzon</t>
-  </si>
-  <si>
-    <t>Chrisse</t>
-  </si>
-  <si>
-    <t>crivenzon1c@163.com</t>
-  </si>
-  <si>
-    <t>Rockall</t>
-  </si>
-  <si>
-    <t>Arley</t>
-  </si>
-  <si>
-    <t>arockall1d@nationalgeographic.com</t>
-  </si>
-  <si>
     <t>Proin eu mi. Nulla ac enim. In tempor, turpis nec euismod scelerisque, quam turpis adipiscing lorem, vitae mattis nibh ligula nec sem. Duis aliquam convallis nunc. Proin at turpis a pede posuere nonummy. Integer non velit. Donec diam neque, vestibulum eget, vulputate ut, ultrices vel, augue. Vestibulum ante ipsum primis in faucibus orci luctus et ultrices posuere cubilia Curae; Donec pharetra, magna vestibulum aliquet ultrices, erat tortor sollicitudin mi, sit amet lobortis sapien sapien non mi. Integer ac neque. Duis bibendum.</t>
   </si>
   <si>
@@ -823,12 +495,21 @@
   </si>
   <si>
     <t>MS</t>
+  </si>
+  <si>
+    <t>FE</t>
+  </si>
+  <si>
+    <t>TitleId</t>
+  </si>
+  <si>
+    <t>FullName</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -866,7 +547,9 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="Invisible" pivot="0" table="0" count="0" xr9:uid="{DC31A8A9-287D-4D6F-ABC4-F08A60369751}"/>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1177,8 +860,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09E4914E-E364-492C-A418-E11389129FC0}">
   <dimension ref="A1:F45"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="F39" sqref="F39"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:F45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1186,7 +869,7 @@
     <col min="1" max="1" width="2.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="39.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="37.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="34.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.85546875" bestFit="1" customWidth="1"/>
   </cols>
@@ -1223,6 +906,10 @@
         <f>CONCATENATE(E2, "_sd")</f>
         <v>Addiction_sd</v>
       </c>
+      <c r="D2" t="str">
+        <f ca="1">VLOOKUP(Blogs!$D2,Authors!$A$2:$F$16,6,FALSE)</f>
+        <v>Emyle Britee, MS</v>
+      </c>
       <c r="E2" t="s">
         <v>6</v>
       </c>
@@ -1243,6 +930,10 @@
         <f t="shared" ref="C3:C45" si="1">CONCATENATE(E3, "_sd")</f>
         <v>Allergy_sd</v>
       </c>
+      <c r="D3" t="str">
+        <f ca="1">VLOOKUP(Blogs!$D3,Authors!$A$2:$F$16,6,FALSE)</f>
+        <v>Maitilde Shead, RN</v>
+      </c>
       <c r="E3" t="s">
         <v>7</v>
       </c>
@@ -1263,6 +954,10 @@
         <f t="shared" si="1"/>
         <v>Autism_sd</v>
       </c>
+      <c r="D4" t="str">
+        <f ca="1">VLOOKUP(Blogs!$D4,Authors!$A$2:$F$16,6,FALSE)</f>
+        <v>Putnem Morphet, PhD</v>
+      </c>
       <c r="E4" t="s">
         <v>8</v>
       </c>
@@ -1283,6 +978,10 @@
         <f t="shared" si="1"/>
         <v>Buckeye Stories_sd</v>
       </c>
+      <c r="D5" t="str">
+        <f ca="1">VLOOKUP(Blogs!$D5,Authors!$A$2:$F$16,6,FALSE)</f>
+        <v>Lawton Basden, RN</v>
+      </c>
       <c r="E5" t="s">
         <v>9</v>
       </c>
@@ -1303,6 +1002,10 @@
         <f t="shared" si="1"/>
         <v>Burn and Wound_sd</v>
       </c>
+      <c r="D6" t="str">
+        <f ca="1">VLOOKUP(Blogs!$D6,Authors!$A$2:$F$16,6,FALSE)</f>
+        <v>Clarisse Wintour, PhD</v>
+      </c>
       <c r="E6" t="s">
         <v>10</v>
       </c>
@@ -1323,6 +1026,10 @@
         <f t="shared" si="1"/>
         <v>Cancer_sd</v>
       </c>
+      <c r="D7" t="str">
+        <f ca="1">VLOOKUP(Blogs!$D7,Authors!$A$2:$F$16,6,FALSE)</f>
+        <v>Dorry Djorevic, LISW</v>
+      </c>
       <c r="E7" t="s">
         <v>11</v>
       </c>
@@ -1343,6 +1050,10 @@
         <f t="shared" si="1"/>
         <v>Cognitive and Memory Disorders_sd</v>
       </c>
+      <c r="D8" t="str">
+        <f ca="1">VLOOKUP(Blogs!$D8,Authors!$A$2:$F$16,6,FALSE)</f>
+        <v>Putnem Morphet, PhD</v>
+      </c>
       <c r="E8" t="s">
         <v>12</v>
       </c>
@@ -1363,6 +1074,10 @@
         <f t="shared" si="1"/>
         <v>Dermatology_sd</v>
       </c>
+      <c r="D9" t="str">
+        <f ca="1">VLOOKUP(Blogs!$D9,Authors!$A$2:$F$16,6,FALSE)</f>
+        <v>Clarisse Wintour, PhD</v>
+      </c>
       <c r="E9" t="s">
         <v>13</v>
       </c>
@@ -1383,6 +1098,10 @@
         <f t="shared" si="1"/>
         <v>Diabetes_sd</v>
       </c>
+      <c r="D10" t="str">
+        <f ca="1">VLOOKUP(Blogs!$D10,Authors!$A$2:$F$16,6,FALSE)</f>
+        <v>Clarisse Wintour, PhD</v>
+      </c>
       <c r="E10" t="s">
         <v>14</v>
       </c>
@@ -1403,6 +1122,10 @@
         <f t="shared" si="1"/>
         <v>Digestive Diseases_sd</v>
       </c>
+      <c r="D11" t="str">
+        <f ca="1">VLOOKUP(Blogs!$D11,Authors!$A$2:$F$16,6,FALSE)</f>
+        <v>Analise Gargett, PharmD</v>
+      </c>
       <c r="E11" t="s">
         <v>15</v>
       </c>
@@ -1423,6 +1146,10 @@
         <f t="shared" si="1"/>
         <v>Ear Nose and Throat_sd</v>
       </c>
+      <c r="D12" t="str">
+        <f ca="1">VLOOKUP(Blogs!$D12,Authors!$A$2:$F$16,6,FALSE)</f>
+        <v>Trudi Aujouanet, MD</v>
+      </c>
       <c r="E12" t="s">
         <v>16</v>
       </c>
@@ -1443,6 +1170,10 @@
         <f t="shared" si="1"/>
         <v>Emergency Medicine_sd</v>
       </c>
+      <c r="D13" t="str">
+        <f ca="1">VLOOKUP(Blogs!$D13,Authors!$A$2:$F$16,6,FALSE)</f>
+        <v>Talia Harower, D(ABMM)</v>
+      </c>
       <c r="E13" t="s">
         <v>17</v>
       </c>
@@ -1463,6 +1194,10 @@
         <f t="shared" si="1"/>
         <v>Endocrinology_sd</v>
       </c>
+      <c r="D14" t="str">
+        <f ca="1">VLOOKUP(Blogs!$D14,Authors!$A$2:$F$16,6,FALSE)</f>
+        <v>Analise Gargett, PharmD</v>
+      </c>
       <c r="E14" t="s">
         <v>18</v>
       </c>
@@ -1483,6 +1218,10 @@
         <f t="shared" si="1"/>
         <v>Eye Care_sd</v>
       </c>
+      <c r="D15" t="str">
+        <f ca="1">VLOOKUP(Blogs!$D15,Authors!$A$2:$F$16,6,FALSE)</f>
+        <v>Maitilde Shead, RN</v>
+      </c>
       <c r="E15" t="s">
         <v>47</v>
       </c>
@@ -1503,6 +1242,10 @@
         <f t="shared" si="1"/>
         <v>Family_sd</v>
       </c>
+      <c r="D16" t="str">
+        <f ca="1">VLOOKUP(Blogs!$D16,Authors!$A$2:$F$16,6,FALSE)</f>
+        <v>Maitilde Shead, RN</v>
+      </c>
       <c r="E16" t="s">
         <v>19</v>
       </c>
@@ -1523,6 +1266,10 @@
         <f t="shared" si="1"/>
         <v>Fitness_sd</v>
       </c>
+      <c r="D17" t="str">
+        <f ca="1">VLOOKUP(Blogs!$D17,Authors!$A$2:$F$16,6,FALSE)</f>
+        <v>Clarisse Wintour, PhD</v>
+      </c>
       <c r="E17" t="s">
         <v>20</v>
       </c>
@@ -1543,6 +1290,10 @@
         <f t="shared" si="1"/>
         <v>Geriatrics_sd</v>
       </c>
+      <c r="D18" t="str">
+        <f ca="1">VLOOKUP(Blogs!$D18,Authors!$A$2:$F$16,6,FALSE)</f>
+        <v>Analise Gargett, PharmD</v>
+      </c>
       <c r="E18" t="s">
         <v>21</v>
       </c>
@@ -1563,6 +1314,10 @@
         <f t="shared" si="1"/>
         <v>Health and Wellness_sd</v>
       </c>
+      <c r="D19" t="str">
+        <f ca="1">VLOOKUP(Blogs!$D19,Authors!$A$2:$F$16,6,FALSE)</f>
+        <v>Analise Gargett, PharmD</v>
+      </c>
       <c r="E19" t="s">
         <v>22</v>
       </c>
@@ -1583,6 +1338,10 @@
         <f>CONCATENATE(E20, "_sd_1")</f>
         <v>Health and Wellness_sd_1</v>
       </c>
+      <c r="D20" t="str">
+        <f ca="1">VLOOKUP(Blogs!$D20,Authors!$A$2:$F$16,6,FALSE)</f>
+        <v>Analise Gargett, PharmD</v>
+      </c>
       <c r="E20" t="s">
         <v>22</v>
       </c>
@@ -1603,6 +1362,10 @@
         <f t="shared" si="1"/>
         <v>Healthy Eating_sd</v>
       </c>
+      <c r="D21" t="str">
+        <f ca="1">VLOOKUP(Blogs!$D21,Authors!$A$2:$F$16,6,FALSE)</f>
+        <v>Lawton Basden, RN</v>
+      </c>
       <c r="E21" t="s">
         <v>23</v>
       </c>
@@ -1623,6 +1386,10 @@
         <f t="shared" si="1"/>
         <v>Hearing Loss_sd</v>
       </c>
+      <c r="D22" t="str">
+        <f ca="1">VLOOKUP(Blogs!$D22,Authors!$A$2:$F$16,6,FALSE)</f>
+        <v>Emyle Britee, MS</v>
+      </c>
       <c r="E22" t="s">
         <v>24</v>
       </c>
@@ -1643,6 +1410,10 @@
         <f t="shared" si="1"/>
         <v>Heart and Vascular Health_sd</v>
       </c>
+      <c r="D23" t="str">
+        <f ca="1">VLOOKUP(Blogs!$D23,Authors!$A$2:$F$16,6,FALSE)</f>
+        <v>Lawton Basden, RN</v>
+      </c>
       <c r="E23" t="s">
         <v>25</v>
       </c>
@@ -1663,6 +1434,10 @@
         <f t="shared" si="1"/>
         <v>Infectious Diseases_sd</v>
       </c>
+      <c r="D24" t="str">
+        <f ca="1">VLOOKUP(Blogs!$D24,Authors!$A$2:$F$16,6,FALSE)</f>
+        <v>Putnem Morphet, PhD</v>
+      </c>
       <c r="E24" t="s">
         <v>26</v>
       </c>
@@ -1683,6 +1458,10 @@
         <f t="shared" si="1"/>
         <v>Integrative Medicine_sd</v>
       </c>
+      <c r="D25" t="str">
+        <f ca="1">VLOOKUP(Blogs!$D25,Authors!$A$2:$F$16,6,FALSE)</f>
+        <v>Emyle Britee, MS</v>
+      </c>
       <c r="E25" t="s">
         <v>27</v>
       </c>
@@ -1703,6 +1482,10 @@
         <f t="shared" si="1"/>
         <v>Lung and Pulmonary_sd</v>
       </c>
+      <c r="D26" t="str">
+        <f ca="1">VLOOKUP(Blogs!$D26,Authors!$A$2:$F$16,6,FALSE)</f>
+        <v>Clarisse Wintour, PhD</v>
+      </c>
       <c r="E26" t="s">
         <v>28</v>
       </c>
@@ -1723,6 +1506,10 @@
         <f t="shared" si="1"/>
         <v>Mental and Behavioral Health_sd</v>
       </c>
+      <c r="D27" t="str">
+        <f ca="1">VLOOKUP(Blogs!$D27,Authors!$A$2:$F$16,6,FALSE)</f>
+        <v>Putnem Morphet, PhD</v>
+      </c>
       <c r="E27" t="s">
         <v>29</v>
       </c>
@@ -1743,6 +1530,10 @@
         <f t="shared" si="1"/>
         <v>MyChart_sd</v>
       </c>
+      <c r="D28" t="str">
+        <f ca="1">VLOOKUP(Blogs!$D28,Authors!$A$2:$F$16,6,FALSE)</f>
+        <v>Analise Gargett, PharmD</v>
+      </c>
       <c r="E28" t="s">
         <v>30</v>
       </c>
@@ -1763,6 +1554,10 @@
         <f t="shared" si="1"/>
         <v>Neurological Institute_sd</v>
       </c>
+      <c r="D29" t="str">
+        <f ca="1">VLOOKUP(Blogs!$D29,Authors!$A$2:$F$16,6,FALSE)</f>
+        <v>Analise Gargett, PharmD</v>
+      </c>
       <c r="E29" t="s">
         <v>48</v>
       </c>
@@ -1783,6 +1578,10 @@
         <f t="shared" si="1"/>
         <v>Nursing_sd</v>
       </c>
+      <c r="D30" t="str">
+        <f ca="1">VLOOKUP(Blogs!$D30,Authors!$A$2:$F$16,6,FALSE)</f>
+        <v>Maitilde Shead, RN</v>
+      </c>
       <c r="E30" t="s">
         <v>31</v>
       </c>
@@ -1803,6 +1602,10 @@
         <f t="shared" si="1"/>
         <v>Orthopedics_sd</v>
       </c>
+      <c r="D31" t="str">
+        <f ca="1">VLOOKUP(Blogs!$D31,Authors!$A$2:$F$16,6,FALSE)</f>
+        <v>Putnem Morphet, PhD</v>
+      </c>
       <c r="E31" t="s">
         <v>32</v>
       </c>
@@ -1823,6 +1626,10 @@
         <f t="shared" si="1"/>
         <v>Physical Medicine and Rehabilitation_sd</v>
       </c>
+      <c r="D32" t="str">
+        <f ca="1">VLOOKUP(Blogs!$D32,Authors!$A$2:$F$16,6,FALSE)</f>
+        <v>Trudi Aujouanet, MD</v>
+      </c>
       <c r="E32" t="s">
         <v>33</v>
       </c>
@@ -1843,6 +1650,10 @@
         <f t="shared" si="1"/>
         <v>Plastic Surgery_sd</v>
       </c>
+      <c r="D33" t="str">
+        <f ca="1">VLOOKUP(Blogs!$D33,Authors!$A$2:$F$16,6,FALSE)</f>
+        <v>Putnem Morphet, PhD</v>
+      </c>
       <c r="E33" t="s">
         <v>34</v>
       </c>
@@ -1863,6 +1674,10 @@
         <f t="shared" si="1"/>
         <v>Primary Care_sd</v>
       </c>
+      <c r="D34" t="str">
+        <f ca="1">VLOOKUP(Blogs!$D34,Authors!$A$2:$F$16,6,FALSE)</f>
+        <v>Putnem Morphet, PhD</v>
+      </c>
       <c r="E34" t="s">
         <v>35</v>
       </c>
@@ -1883,6 +1698,10 @@
         <f t="shared" si="1"/>
         <v>Research_sd</v>
       </c>
+      <c r="D35" t="str">
+        <f ca="1">VLOOKUP(Blogs!$D35,Authors!$A$2:$F$16,6,FALSE)</f>
+        <v>Maitilde Shead, RN</v>
+      </c>
       <c r="E35" t="s">
         <v>36</v>
       </c>
@@ -1903,6 +1722,10 @@
         <f t="shared" si="1"/>
         <v>Rheumatology_sd</v>
       </c>
+      <c r="D36" t="str">
+        <f ca="1">VLOOKUP(Blogs!$D36,Authors!$A$2:$F$16,6,FALSE)</f>
+        <v>Dorry Djorevic, LISW</v>
+      </c>
       <c r="E36" t="s">
         <v>37</v>
       </c>
@@ -1923,6 +1746,10 @@
         <f t="shared" si="1"/>
         <v>Sleep_sd</v>
       </c>
+      <c r="D37" t="str">
+        <f ca="1">VLOOKUP(Blogs!$D37,Authors!$A$2:$F$16,6,FALSE)</f>
+        <v>Talia Harower, D(ABMM)</v>
+      </c>
       <c r="E37" t="s">
         <v>38</v>
       </c>
@@ -1943,6 +1770,10 @@
         <f t="shared" si="1"/>
         <v>Sports Medicine_sd</v>
       </c>
+      <c r="D38" t="str">
+        <f ca="1">VLOOKUP(Blogs!$D38,Authors!$A$2:$F$16,6,FALSE)</f>
+        <v>Trudi Aujouanet, MD</v>
+      </c>
       <c r="E38" t="s">
         <v>39</v>
       </c>
@@ -1963,6 +1794,10 @@
         <f t="shared" si="1"/>
         <v>Stress Management_sd</v>
       </c>
+      <c r="D39" t="str">
+        <f ca="1">VLOOKUP(Blogs!$D39,Authors!$A$2:$F$16,6,FALSE)</f>
+        <v>Putnem Morphet, PhD</v>
+      </c>
       <c r="E39" t="s">
         <v>40</v>
       </c>
@@ -1983,6 +1818,10 @@
         <f t="shared" si="1"/>
         <v>Tech and Innovation_sd</v>
       </c>
+      <c r="D40" t="str">
+        <f ca="1">VLOOKUP(Blogs!$D40,Authors!$A$2:$F$16,6,FALSE)</f>
+        <v>Clarisse Wintour, PhD</v>
+      </c>
       <c r="E40" t="s">
         <v>41</v>
       </c>
@@ -2003,6 +1842,10 @@
         <f t="shared" si="1"/>
         <v>Transplant_sd</v>
       </c>
+      <c r="D41" t="str">
+        <f ca="1">VLOOKUP(Blogs!$D41,Authors!$A$2:$F$16,6,FALSE)</f>
+        <v>Clarisse Wintour, PhD</v>
+      </c>
       <c r="E41" t="s">
         <v>42</v>
       </c>
@@ -2023,6 +1866,10 @@
         <f t="shared" si="1"/>
         <v>Urology_sd</v>
       </c>
+      <c r="D42" t="str">
+        <f ca="1">VLOOKUP(Blogs!$D42,Authors!$A$2:$F$16,6,FALSE)</f>
+        <v>Talia Harower, D(ABMM)</v>
+      </c>
       <c r="E42" t="s">
         <v>43</v>
       </c>
@@ -2043,6 +1890,10 @@
         <f t="shared" si="1"/>
         <v>Weight Management_sd</v>
       </c>
+      <c r="D43" t="str">
+        <f ca="1">VLOOKUP(Blogs!$D43,Authors!$A$2:$F$16,6,FALSE)</f>
+        <v>Lawton Basden, RN</v>
+      </c>
       <c r="E43" t="s">
         <v>44</v>
       </c>
@@ -2063,6 +1914,10 @@
         <f t="shared" si="1"/>
         <v>Women and Infants_sd</v>
       </c>
+      <c r="D44" t="str">
+        <f ca="1">VLOOKUP(Blogs!$D44,Authors!$A$2:$F$16,6,FALSE)</f>
+        <v>Lawton Basden, RN</v>
+      </c>
       <c r="E44" t="s">
         <v>45</v>
       </c>
@@ -2082,6 +1937,10 @@
       <c r="C45" t="str">
         <f t="shared" si="1"/>
         <v>Womens Health_sd</v>
+      </c>
+      <c r="D45" t="str">
+        <f ca="1">VLOOKUP(Blogs!$D45,Authors!$A$2:$F$16,6,FALSE)</f>
+        <v>Talia Harower, D(ABMM)</v>
       </c>
       <c r="E45" t="s">
         <v>46</v>
@@ -2099,8 +1958,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD98D479-EDA0-489A-9E07-8C27F6ED29A4}">
   <dimension ref="A1:G45"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="E47" sqref="E47"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2149,11 +2008,15 @@
         <f>CONCATENATE(E2, "_sd")</f>
         <v>Addiction_sd</v>
       </c>
+      <c r="D2">
+        <f ca="1">_xlfn.CEILING.MATH(RAND()*9+1)</f>
+        <v>9</v>
+      </c>
       <c r="E2" t="s">
         <v>6</v>
       </c>
       <c r="F2" t="s">
-        <v>209</v>
+        <v>100</v>
       </c>
       <c r="G2" s="1">
         <v>43650.741631944446</v>
@@ -2172,11 +2035,15 @@
         <f t="shared" ref="C3:C45" si="1">CONCATENATE(E3, "_sd")</f>
         <v>Allergy_sd</v>
       </c>
+      <c r="D3">
+        <f t="shared" ref="D3:D45" ca="1" si="2">_xlfn.CEILING.MATH(RAND()*9+1)</f>
+        <v>7</v>
+      </c>
       <c r="E3" t="s">
         <v>7</v>
       </c>
       <c r="F3" t="s">
-        <v>210</v>
+        <v>101</v>
       </c>
       <c r="G3" s="1">
         <v>43983.622939814813</v>
@@ -2184,7 +2051,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
-        <f t="shared" ref="A4:A45" si="2">1+A3</f>
+        <f t="shared" ref="A4:A45" si="3">1+A3</f>
         <v>3</v>
       </c>
       <c r="B4" t="str">
@@ -2194,12 +2061,16 @@
       <c r="C4" t="str">
         <f t="shared" si="1"/>
         <v>Autism_sd</v>
+      </c>
+      <c r="D4">
+        <f t="shared" ca="1" si="2"/>
+        <v>5</v>
       </c>
       <c r="E4" t="s">
         <v>8</v>
       </c>
       <c r="F4" t="s">
-        <v>211</v>
+        <v>102</v>
       </c>
       <c r="G4" s="1">
         <v>44052.233229166668</v>
@@ -2207,7 +2078,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="B5" t="str">
@@ -2217,12 +2088,16 @@
       <c r="C5" t="str">
         <f t="shared" si="1"/>
         <v>Buckeye Stories_sd</v>
+      </c>
+      <c r="D5">
+        <f t="shared" ca="1" si="2"/>
+        <v>6</v>
       </c>
       <c r="E5" t="s">
         <v>9</v>
       </c>
       <c r="F5" t="s">
-        <v>212</v>
+        <v>103</v>
       </c>
       <c r="G5" s="1">
         <v>43953.700960648152</v>
@@ -2230,7 +2105,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="B6" t="str">
@@ -2240,12 +2115,16 @@
       <c r="C6" t="str">
         <f t="shared" si="1"/>
         <v>Burn and Wound_sd</v>
+      </c>
+      <c r="D6">
+        <f t="shared" ca="1" si="2"/>
+        <v>10</v>
       </c>
       <c r="E6" t="s">
         <v>10</v>
       </c>
       <c r="F6" t="s">
-        <v>213</v>
+        <v>104</v>
       </c>
       <c r="G6" s="1">
         <v>44503.872523148151</v>
@@ -2253,7 +2132,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
       <c r="B7" t="str">
@@ -2263,12 +2142,16 @@
       <c r="C7" t="str">
         <f t="shared" si="1"/>
         <v>Cancer_sd</v>
+      </c>
+      <c r="D7">
+        <f t="shared" ca="1" si="2"/>
+        <v>3</v>
       </c>
       <c r="E7" t="s">
         <v>11</v>
       </c>
       <c r="F7" t="s">
-        <v>214</v>
+        <v>105</v>
       </c>
       <c r="G7" s="1">
         <v>44436.837754629632</v>
@@ -2276,7 +2159,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>7</v>
       </c>
       <c r="B8" t="str">
@@ -2286,12 +2169,16 @@
       <c r="C8" t="str">
         <f t="shared" si="1"/>
         <v>Cognitive and Memory Disorders_sd</v>
+      </c>
+      <c r="D8">
+        <f t="shared" ca="1" si="2"/>
+        <v>5</v>
       </c>
       <c r="E8" t="s">
         <v>12</v>
       </c>
       <c r="F8" t="s">
-        <v>215</v>
+        <v>106</v>
       </c>
       <c r="G8" s="1">
         <v>43883.556168981479</v>
@@ -2299,7 +2186,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="B9" t="str">
@@ -2309,12 +2196,16 @@
       <c r="C9" t="str">
         <f t="shared" si="1"/>
         <v>Dermatology_sd</v>
+      </c>
+      <c r="D9">
+        <f t="shared" ca="1" si="2"/>
+        <v>10</v>
       </c>
       <c r="E9" t="s">
         <v>13</v>
       </c>
       <c r="F9" t="s">
-        <v>216</v>
+        <v>107</v>
       </c>
       <c r="G9" s="1">
         <v>44342.035775462966</v>
@@ -2322,7 +2213,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>9</v>
       </c>
       <c r="B10" t="str">
@@ -2332,12 +2223,16 @@
       <c r="C10" t="str">
         <f t="shared" si="1"/>
         <v>Diabetes_sd</v>
+      </c>
+      <c r="D10">
+        <f t="shared" ca="1" si="2"/>
+        <v>10</v>
       </c>
       <c r="E10" t="s">
         <v>14</v>
       </c>
       <c r="F10" t="s">
-        <v>217</v>
+        <v>108</v>
       </c>
       <c r="G10" s="1">
         <v>43981.434108796297</v>
@@ -2345,7 +2240,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
       <c r="B11" t="str">
@@ -2355,12 +2250,16 @@
       <c r="C11" t="str">
         <f t="shared" si="1"/>
         <v>Digestive Diseases_sd</v>
+      </c>
+      <c r="D11">
+        <f t="shared" ca="1" si="2"/>
+        <v>4</v>
       </c>
       <c r="E11" t="s">
         <v>15</v>
       </c>
       <c r="F11" t="s">
-        <v>218</v>
+        <v>109</v>
       </c>
       <c r="G11" s="1">
         <v>44439.301180555558</v>
@@ -2368,7 +2267,7 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>11</v>
       </c>
       <c r="B12" t="str">
@@ -2378,12 +2277,16 @@
       <c r="C12" t="str">
         <f t="shared" si="1"/>
         <v>Ear Nose and Throat_sd</v>
+      </c>
+      <c r="D12">
+        <f t="shared" ca="1" si="2"/>
+        <v>2</v>
       </c>
       <c r="E12" t="s">
         <v>16</v>
       </c>
       <c r="F12" t="s">
-        <v>219</v>
+        <v>110</v>
       </c>
       <c r="G12" s="1">
         <v>43839.48810185185</v>
@@ -2391,7 +2294,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>12</v>
       </c>
       <c r="B13" t="str">
@@ -2401,12 +2304,16 @@
       <c r="C13" t="str">
         <f t="shared" si="1"/>
         <v>Emergency Medicine_sd</v>
+      </c>
+      <c r="D13">
+        <f t="shared" ca="1" si="2"/>
+        <v>8</v>
       </c>
       <c r="E13" t="s">
         <v>17</v>
       </c>
       <c r="F13" t="s">
-        <v>220</v>
+        <v>111</v>
       </c>
       <c r="G13" s="1">
         <v>44165.725937499999</v>
@@ -2414,7 +2321,7 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>13</v>
       </c>
       <c r="B14" t="str">
@@ -2424,12 +2331,16 @@
       <c r="C14" t="str">
         <f t="shared" si="1"/>
         <v>Endocrinology_sd</v>
+      </c>
+      <c r="D14">
+        <f t="shared" ca="1" si="2"/>
+        <v>4</v>
       </c>
       <c r="E14" t="s">
         <v>18</v>
       </c>
       <c r="F14" t="s">
-        <v>221</v>
+        <v>112</v>
       </c>
       <c r="G14" s="1">
         <v>43789.461516203701</v>
@@ -2437,7 +2348,7 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>14</v>
       </c>
       <c r="B15" t="str">
@@ -2447,12 +2358,16 @@
       <c r="C15" t="str">
         <f t="shared" si="1"/>
         <v>Eye Care_sd</v>
+      </c>
+      <c r="D15">
+        <f t="shared" ca="1" si="2"/>
+        <v>7</v>
       </c>
       <c r="E15" t="s">
         <v>47</v>
       </c>
       <c r="F15" t="s">
-        <v>222</v>
+        <v>113</v>
       </c>
       <c r="G15" s="1">
         <v>44378.034907407404</v>
@@ -2460,7 +2375,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>15</v>
       </c>
       <c r="B16" t="str">
@@ -2470,12 +2385,16 @@
       <c r="C16" t="str">
         <f t="shared" si="1"/>
         <v>Family_sd</v>
+      </c>
+      <c r="D16">
+        <f t="shared" ca="1" si="2"/>
+        <v>7</v>
       </c>
       <c r="E16" t="s">
         <v>19</v>
       </c>
       <c r="F16" t="s">
-        <v>223</v>
+        <v>114</v>
       </c>
       <c r="G16" s="1">
         <v>43929.743101851855</v>
@@ -2483,7 +2402,7 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>16</v>
       </c>
       <c r="B17" t="str">
@@ -2493,12 +2412,16 @@
       <c r="C17" t="str">
         <f t="shared" si="1"/>
         <v>Fitness_sd</v>
+      </c>
+      <c r="D17">
+        <f t="shared" ca="1" si="2"/>
+        <v>10</v>
       </c>
       <c r="E17" t="s">
         <v>20</v>
       </c>
       <c r="F17" t="s">
-        <v>224</v>
+        <v>115</v>
       </c>
       <c r="G17" s="1">
         <v>44082.219421296293</v>
@@ -2506,7 +2429,7 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>17</v>
       </c>
       <c r="B18" t="str">
@@ -2516,12 +2439,16 @@
       <c r="C18" t="str">
         <f t="shared" si="1"/>
         <v>Geriatrics_sd</v>
+      </c>
+      <c r="D18">
+        <f t="shared" ca="1" si="2"/>
+        <v>4</v>
       </c>
       <c r="E18" t="s">
         <v>21</v>
       </c>
       <c r="F18" t="s">
-        <v>225</v>
+        <v>116</v>
       </c>
       <c r="G18" s="1">
         <v>44683.857743055552</v>
@@ -2529,7 +2456,7 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>18</v>
       </c>
       <c r="B19" t="str">
@@ -2540,11 +2467,15 @@
         <f t="shared" si="1"/>
         <v>Health and Wellness_sd</v>
       </c>
+      <c r="D19">
+        <f t="shared" ca="1" si="2"/>
+        <v>4</v>
+      </c>
       <c r="E19" t="s">
         <v>22</v>
       </c>
       <c r="F19" t="s">
-        <v>226</v>
+        <v>117</v>
       </c>
       <c r="G19" s="1">
         <v>43960.36509259259</v>
@@ -2552,7 +2483,7 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>19</v>
       </c>
       <c r="B20" t="str">
@@ -2563,11 +2494,15 @@
         <f>CONCATENATE(E20, "_sd_1")</f>
         <v>Health and Wellness_sd_1</v>
       </c>
+      <c r="D20">
+        <f t="shared" ca="1" si="2"/>
+        <v>4</v>
+      </c>
       <c r="E20" t="s">
         <v>22</v>
       </c>
       <c r="F20" t="s">
-        <v>227</v>
+        <v>118</v>
       </c>
       <c r="G20" s="1">
         <v>44440.085810185185</v>
@@ -2575,7 +2510,7 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>20</v>
       </c>
       <c r="B21" t="str">
@@ -2585,12 +2520,16 @@
       <c r="C21" t="str">
         <f t="shared" si="1"/>
         <v>Healthy Eating_sd</v>
+      </c>
+      <c r="D21">
+        <f t="shared" ca="1" si="2"/>
+        <v>6</v>
       </c>
       <c r="E21" t="s">
         <v>23</v>
       </c>
       <c r="F21" t="s">
-        <v>228</v>
+        <v>119</v>
       </c>
       <c r="G21" s="1">
         <v>44413.808518518519</v>
@@ -2598,7 +2537,7 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>21</v>
       </c>
       <c r="B22" t="str">
@@ -2608,12 +2547,16 @@
       <c r="C22" t="str">
         <f t="shared" si="1"/>
         <v>Hearing Loss_sd</v>
+      </c>
+      <c r="D22">
+        <f t="shared" ca="1" si="2"/>
+        <v>9</v>
       </c>
       <c r="E22" t="s">
         <v>24</v>
       </c>
       <c r="F22" t="s">
-        <v>229</v>
+        <v>120</v>
       </c>
       <c r="G22" s="1">
         <v>44515.085358796299</v>
@@ -2621,7 +2564,7 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>22</v>
       </c>
       <c r="B23" t="str">
@@ -2631,12 +2574,16 @@
       <c r="C23" t="str">
         <f t="shared" si="1"/>
         <v>Heart and Vascular Health_sd</v>
+      </c>
+      <c r="D23">
+        <f t="shared" ca="1" si="2"/>
+        <v>6</v>
       </c>
       <c r="E23" t="s">
         <v>25</v>
       </c>
       <c r="F23" t="s">
-        <v>230</v>
+        <v>121</v>
       </c>
       <c r="G23" s="1">
         <v>43844.797719907408</v>
@@ -2644,7 +2591,7 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>23</v>
       </c>
       <c r="B24" t="str">
@@ -2654,12 +2601,16 @@
       <c r="C24" t="str">
         <f t="shared" si="1"/>
         <v>Infectious Diseases_sd</v>
+      </c>
+      <c r="D24">
+        <f t="shared" ca="1" si="2"/>
+        <v>5</v>
       </c>
       <c r="E24" t="s">
         <v>26</v>
       </c>
       <c r="F24" t="s">
-        <v>231</v>
+        <v>122</v>
       </c>
       <c r="G24" s="1">
         <v>44647.730243055557</v>
@@ -2667,7 +2618,7 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>24</v>
       </c>
       <c r="B25" t="str">
@@ -2677,12 +2628,16 @@
       <c r="C25" t="str">
         <f t="shared" si="1"/>
         <v>Integrative Medicine_sd</v>
+      </c>
+      <c r="D25">
+        <f t="shared" ca="1" si="2"/>
+        <v>9</v>
       </c>
       <c r="E25" t="s">
         <v>27</v>
       </c>
       <c r="F25" t="s">
-        <v>232</v>
+        <v>123</v>
       </c>
       <c r="G25" s="1">
         <v>43683.203715277778</v>
@@ -2690,7 +2645,7 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>25</v>
       </c>
       <c r="B26" t="str">
@@ -2700,12 +2655,16 @@
       <c r="C26" t="str">
         <f t="shared" si="1"/>
         <v>Lung and Pulmonary_sd</v>
+      </c>
+      <c r="D26">
+        <f t="shared" ca="1" si="2"/>
+        <v>10</v>
       </c>
       <c r="E26" t="s">
         <v>28</v>
       </c>
       <c r="F26" t="s">
-        <v>233</v>
+        <v>124</v>
       </c>
       <c r="G26" s="1">
         <v>44711.372303240743</v>
@@ -2713,7 +2672,7 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>26</v>
       </c>
       <c r="B27" t="str">
@@ -2723,12 +2682,16 @@
       <c r="C27" t="str">
         <f t="shared" si="1"/>
         <v>Mental and Behavioral Health_sd</v>
+      </c>
+      <c r="D27">
+        <f t="shared" ca="1" si="2"/>
+        <v>5</v>
       </c>
       <c r="E27" t="s">
         <v>29</v>
       </c>
       <c r="F27" t="s">
-        <v>234</v>
+        <v>125</v>
       </c>
       <c r="G27" s="1">
         <v>44537.602222222224</v>
@@ -2736,7 +2699,7 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>27</v>
       </c>
       <c r="B28" t="str">
@@ -2746,12 +2709,16 @@
       <c r="C28" t="str">
         <f t="shared" si="1"/>
         <v>MyChart_sd</v>
+      </c>
+      <c r="D28">
+        <f t="shared" ca="1" si="2"/>
+        <v>4</v>
       </c>
       <c r="E28" t="s">
         <v>30</v>
       </c>
       <c r="F28" t="s">
-        <v>235</v>
+        <v>126</v>
       </c>
       <c r="G28" s="1">
         <v>43754.51321759259</v>
@@ -2759,7 +2726,7 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>28</v>
       </c>
       <c r="B29" t="str">
@@ -2769,12 +2736,16 @@
       <c r="C29" t="str">
         <f t="shared" si="1"/>
         <v>Neurological Institute_sd</v>
+      </c>
+      <c r="D29">
+        <f t="shared" ca="1" si="2"/>
+        <v>4</v>
       </c>
       <c r="E29" t="s">
         <v>48</v>
       </c>
       <c r="F29" t="s">
-        <v>236</v>
+        <v>127</v>
       </c>
       <c r="G29" s="1">
         <v>44263.361319444448</v>
@@ -2782,7 +2753,7 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>29</v>
       </c>
       <c r="B30" t="str">
@@ -2792,12 +2763,16 @@
       <c r="C30" t="str">
         <f t="shared" si="1"/>
         <v>Nursing_sd</v>
+      </c>
+      <c r="D30">
+        <f t="shared" ca="1" si="2"/>
+        <v>7</v>
       </c>
       <c r="E30" t="s">
         <v>31</v>
       </c>
       <c r="F30" t="s">
-        <v>237</v>
+        <v>128</v>
       </c>
       <c r="G30" s="1">
         <v>43713.270162037035</v>
@@ -2816,11 +2791,15 @@
         <f t="shared" si="1"/>
         <v>Orthopedics_sd</v>
       </c>
+      <c r="D31">
+        <f t="shared" ca="1" si="2"/>
+        <v>5</v>
+      </c>
       <c r="E31" t="s">
         <v>32</v>
       </c>
       <c r="F31" t="s">
-        <v>238</v>
+        <v>129</v>
       </c>
       <c r="G31" s="1">
         <v>43728.261180555557</v>
@@ -2828,7 +2807,7 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>31</v>
       </c>
       <c r="B32" t="str">
@@ -2838,12 +2817,16 @@
       <c r="C32" t="str">
         <f t="shared" si="1"/>
         <v>Physical Medicine and Rehabilitation_sd</v>
+      </c>
+      <c r="D32">
+        <f t="shared" ca="1" si="2"/>
+        <v>2</v>
       </c>
       <c r="E32" t="s">
         <v>33</v>
       </c>
       <c r="F32" t="s">
-        <v>239</v>
+        <v>130</v>
       </c>
       <c r="G32" s="1">
         <v>44387.354062500002</v>
@@ -2851,7 +2834,7 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>32</v>
       </c>
       <c r="B33" t="str">
@@ -2861,12 +2844,16 @@
       <c r="C33" t="str">
         <f t="shared" si="1"/>
         <v>Plastic Surgery_sd</v>
+      </c>
+      <c r="D33">
+        <f t="shared" ca="1" si="2"/>
+        <v>5</v>
       </c>
       <c r="E33" t="s">
         <v>34</v>
       </c>
       <c r="F33" t="s">
-        <v>240</v>
+        <v>131</v>
       </c>
       <c r="G33" s="1">
         <v>44707.080995370372</v>
@@ -2874,7 +2861,7 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>33</v>
       </c>
       <c r="B34" t="str">
@@ -2884,12 +2871,16 @@
       <c r="C34" t="str">
         <f t="shared" si="1"/>
         <v>Primary Care_sd</v>
+      </c>
+      <c r="D34">
+        <f t="shared" ca="1" si="2"/>
+        <v>5</v>
       </c>
       <c r="E34" t="s">
         <v>35</v>
       </c>
       <c r="F34" t="s">
-        <v>241</v>
+        <v>132</v>
       </c>
       <c r="G34" s="1">
         <v>43892.60765046296</v>
@@ -2897,7 +2888,7 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>34</v>
       </c>
       <c r="B35" t="str">
@@ -2907,12 +2898,16 @@
       <c r="C35" t="str">
         <f t="shared" si="1"/>
         <v>Research_sd</v>
+      </c>
+      <c r="D35">
+        <f t="shared" ca="1" si="2"/>
+        <v>7</v>
       </c>
       <c r="E35" t="s">
         <v>36</v>
       </c>
       <c r="F35" t="s">
-        <v>242</v>
+        <v>133</v>
       </c>
       <c r="G35" s="1">
         <v>43762.497800925928</v>
@@ -2920,7 +2915,7 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>35</v>
       </c>
       <c r="B36" t="str">
@@ -2930,12 +2925,16 @@
       <c r="C36" t="str">
         <f t="shared" si="1"/>
         <v>Rheumatology_sd</v>
+      </c>
+      <c r="D36">
+        <f t="shared" ca="1" si="2"/>
+        <v>3</v>
       </c>
       <c r="E36" t="s">
         <v>37</v>
       </c>
       <c r="F36" t="s">
-        <v>243</v>
+        <v>134</v>
       </c>
       <c r="G36" s="1">
         <v>44580.349097222221</v>
@@ -2943,7 +2942,7 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>36</v>
       </c>
       <c r="B37" t="str">
@@ -2953,12 +2952,16 @@
       <c r="C37" t="str">
         <f t="shared" si="1"/>
         <v>Sleep_sd</v>
+      </c>
+      <c r="D37">
+        <f t="shared" ca="1" si="2"/>
+        <v>8</v>
       </c>
       <c r="E37" t="s">
         <v>38</v>
       </c>
       <c r="F37" t="s">
-        <v>244</v>
+        <v>135</v>
       </c>
       <c r="G37" s="1">
         <v>43760.509976851848</v>
@@ -2966,7 +2969,7 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>37</v>
       </c>
       <c r="B38" t="str">
@@ -2976,12 +2979,16 @@
       <c r="C38" t="str">
         <f t="shared" si="1"/>
         <v>Sports Medicine_sd</v>
+      </c>
+      <c r="D38">
+        <f t="shared" ca="1" si="2"/>
+        <v>2</v>
       </c>
       <c r="E38" t="s">
         <v>39</v>
       </c>
       <c r="F38" t="s">
-        <v>245</v>
+        <v>136</v>
       </c>
       <c r="G38" s="1">
         <v>44588.86146990741</v>
@@ -2989,7 +2996,7 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>38</v>
       </c>
       <c r="B39" t="str">
@@ -2999,12 +3006,16 @@
       <c r="C39" t="str">
         <f t="shared" si="1"/>
         <v>Stress Management_sd</v>
+      </c>
+      <c r="D39">
+        <f t="shared" ca="1" si="2"/>
+        <v>5</v>
       </c>
       <c r="E39" t="s">
         <v>40</v>
       </c>
       <c r="F39" t="s">
-        <v>246</v>
+        <v>137</v>
       </c>
       <c r="G39" s="1">
         <v>44516.732303240744</v>
@@ -3012,7 +3023,7 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>39</v>
       </c>
       <c r="B40" t="str">
@@ -3022,12 +3033,16 @@
       <c r="C40" t="str">
         <f t="shared" si="1"/>
         <v>Tech and Innovation_sd</v>
+      </c>
+      <c r="D40">
+        <f t="shared" ca="1" si="2"/>
+        <v>10</v>
       </c>
       <c r="E40" t="s">
         <v>41</v>
       </c>
       <c r="F40" t="s">
-        <v>247</v>
+        <v>138</v>
       </c>
       <c r="G40" s="1">
         <v>44313.694722222222</v>
@@ -3035,7 +3050,7 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>40</v>
       </c>
       <c r="B41" t="str">
@@ -3045,12 +3060,16 @@
       <c r="C41" t="str">
         <f t="shared" si="1"/>
         <v>Transplant_sd</v>
+      </c>
+      <c r="D41">
+        <f t="shared" ca="1" si="2"/>
+        <v>10</v>
       </c>
       <c r="E41" t="s">
         <v>42</v>
       </c>
       <c r="F41" t="s">
-        <v>248</v>
+        <v>139</v>
       </c>
       <c r="G41" s="1">
         <v>44277.690486111111</v>
@@ -3058,7 +3077,7 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>41</v>
       </c>
       <c r="B42" t="str">
@@ -3068,12 +3087,16 @@
       <c r="C42" t="str">
         <f t="shared" si="1"/>
         <v>Urology_sd</v>
+      </c>
+      <c r="D42">
+        <f t="shared" ca="1" si="2"/>
+        <v>8</v>
       </c>
       <c r="E42" t="s">
         <v>43</v>
       </c>
       <c r="F42" t="s">
-        <v>249</v>
+        <v>140</v>
       </c>
       <c r="G42" s="1">
         <v>43722.768078703702</v>
@@ -3081,7 +3104,7 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>42</v>
       </c>
       <c r="B43" t="str">
@@ -3091,12 +3114,16 @@
       <c r="C43" t="str">
         <f t="shared" si="1"/>
         <v>Weight Management_sd</v>
+      </c>
+      <c r="D43">
+        <f t="shared" ca="1" si="2"/>
+        <v>6</v>
       </c>
       <c r="E43" t="s">
         <v>44</v>
       </c>
       <c r="F43" t="s">
-        <v>250</v>
+        <v>141</v>
       </c>
       <c r="G43" s="1">
         <v>44597.995046296295</v>
@@ -3104,7 +3131,7 @@
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>43</v>
       </c>
       <c r="B44" t="str">
@@ -3114,12 +3141,16 @@
       <c r="C44" t="str">
         <f t="shared" si="1"/>
         <v>Women and Infants_sd</v>
+      </c>
+      <c r="D44">
+        <f t="shared" ca="1" si="2"/>
+        <v>6</v>
       </c>
       <c r="E44" t="s">
         <v>45</v>
       </c>
       <c r="F44" t="s">
-        <v>251</v>
+        <v>142</v>
       </c>
       <c r="G44" s="1">
         <v>43947.205312500002</v>
@@ -3127,7 +3158,7 @@
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>44</v>
       </c>
       <c r="B45" t="str">
@@ -3137,12 +3168,16 @@
       <c r="C45" t="str">
         <f t="shared" si="1"/>
         <v>Womens Health_sd</v>
+      </c>
+      <c r="D45">
+        <f t="shared" ca="1" si="2"/>
+        <v>8</v>
       </c>
       <c r="E45" t="s">
         <v>46</v>
       </c>
       <c r="F45" t="s">
-        <v>252</v>
+        <v>143</v>
       </c>
       <c r="G45" s="1">
         <v>44576.97761574074</v>
@@ -3155,10 +3190,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A34946C6-B7B2-4340-A169-16E0ADD794C5}">
-  <dimension ref="A1:F51"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="F1" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3168,7 +3203,7 @@
     <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="34" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27.28515625" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -3182,13 +3217,13 @@
         <v>50</v>
       </c>
       <c r="D1" t="s">
-        <v>1</v>
+        <v>153</v>
       </c>
       <c r="E1" t="s">
         <v>51</v>
       </c>
       <c r="F1" t="s">
-        <v>55</v>
+        <v>154</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -3197,16 +3232,20 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C2" t="s">
-        <v>60</v>
-      </c>
-      <c r="D2" t="s">
-        <v>253</v>
+        <v>56</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>61</v>
+        <v>57</v>
+      </c>
+      <c r="F2" t="str">
+        <f>C2 &amp; " " &amp; B2 &amp; ", " &amp; VLOOKUP($D2,Titles!$A$2:$B$11,2,FALSE)</f>
+        <v>Auguste Boatwright, MD</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -3215,28 +3254,42 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C3" t="s">
-        <v>63</v>
+        <v>59</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>64</v>
+        <v>60</v>
+      </c>
+      <c r="F3" t="str">
+        <f>C3 &amp; " " &amp; B3 &amp; ", " &amp; VLOOKUP($D3,Titles!$A$2:$B$11,2,FALSE)</f>
+        <v>Trudi Aujouanet, MD</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
-        <f t="shared" ref="A4:A51" si="0">1+A3</f>
+        <f t="shared" ref="A4:A16" si="0">1+A3</f>
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C4" t="s">
-        <v>66</v>
+        <v>62</v>
+      </c>
+      <c r="D4">
+        <v>3</v>
       </c>
       <c r="E4" t="s">
-        <v>67</v>
+        <v>63</v>
+      </c>
+      <c r="F4" t="str">
+        <f>C4 &amp; " " &amp; B4 &amp; ", " &amp; VLOOKUP($D4,Titles!$A$2:$B$11,2,FALSE)</f>
+        <v>Dorry Djorevic, LISW</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -3245,13 +3298,20 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C5" t="s">
-        <v>69</v>
+        <v>65</v>
+      </c>
+      <c r="D5">
+        <v>5</v>
       </c>
       <c r="E5" t="s">
-        <v>70</v>
+        <v>66</v>
+      </c>
+      <c r="F5" t="str">
+        <f>C5 &amp; " " &amp; B5 &amp; ", " &amp; VLOOKUP($D5,Titles!$A$2:$B$11,2,FALSE)</f>
+        <v>Analise Gargett, PharmD</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -3260,13 +3320,20 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C6" t="s">
-        <v>72</v>
+        <v>68</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
       </c>
       <c r="E6" t="s">
-        <v>73</v>
+        <v>69</v>
+      </c>
+      <c r="F6" t="str">
+        <f>C6 &amp; " " &amp; B6 &amp; ", " &amp; VLOOKUP($D6,Titles!$A$2:$B$11,2,FALSE)</f>
+        <v>Putnem Morphet, PhD</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -3275,13 +3342,20 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C7" t="s">
-        <v>75</v>
+        <v>71</v>
+      </c>
+      <c r="D7">
+        <v>4</v>
       </c>
       <c r="E7" t="s">
-        <v>76</v>
+        <v>72</v>
+      </c>
+      <c r="F7" t="str">
+        <f>C7 &amp; " " &amp; B7 &amp; ", " &amp; VLOOKUP($D7,Titles!$A$2:$B$11,2,FALSE)</f>
+        <v>Lawton Basden, RN</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -3290,13 +3364,20 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C8" t="s">
-        <v>78</v>
+        <v>74</v>
+      </c>
+      <c r="D8">
+        <v>4</v>
       </c>
       <c r="E8" t="s">
-        <v>79</v>
+        <v>75</v>
+      </c>
+      <c r="F8" t="str">
+        <f>C8 &amp; " " &amp; B8 &amp; ", " &amp; VLOOKUP($D8,Titles!$A$2:$B$11,2,FALSE)</f>
+        <v>Maitilde Shead, RN</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -3305,13 +3386,20 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C9" t="s">
-        <v>81</v>
+        <v>77</v>
+      </c>
+      <c r="D9">
+        <v>6</v>
       </c>
       <c r="E9" t="s">
-        <v>82</v>
+        <v>78</v>
+      </c>
+      <c r="F9" t="str">
+        <f>C9 &amp; " " &amp; B9 &amp; ", " &amp; VLOOKUP($D9,Titles!$A$2:$B$11,2,FALSE)</f>
+        <v>Talia Harower, D(ABMM)</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -3320,13 +3408,20 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C10" t="s">
-        <v>84</v>
+        <v>80</v>
+      </c>
+      <c r="D10">
+        <v>9</v>
       </c>
       <c r="E10" t="s">
-        <v>85</v>
+        <v>81</v>
+      </c>
+      <c r="F10" t="str">
+        <f>C10 &amp; " " &amp; B10 &amp; ", " &amp; VLOOKUP($D10,Titles!$A$2:$B$11,2,FALSE)</f>
+        <v>Emyle Britee, MS</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -3335,13 +3430,20 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C11" t="s">
-        <v>87</v>
+        <v>83</v>
+      </c>
+      <c r="D11">
+        <v>2</v>
       </c>
       <c r="E11" t="s">
-        <v>88</v>
+        <v>84</v>
+      </c>
+      <c r="F11" t="str">
+        <f>C11 &amp; " " &amp; B11 &amp; ", " &amp; VLOOKUP($D11,Titles!$A$2:$B$11,2,FALSE)</f>
+        <v>Clarisse Wintour, PhD</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -3350,13 +3452,20 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C12" t="s">
-        <v>90</v>
+        <v>86</v>
+      </c>
+      <c r="D12">
+        <v>3</v>
       </c>
       <c r="E12" t="s">
-        <v>91</v>
+        <v>87</v>
+      </c>
+      <c r="F12" t="str">
+        <f>C12 &amp; " " &amp; B12 &amp; ", " &amp; VLOOKUP($D12,Titles!$A$2:$B$11,2,FALSE)</f>
+        <v>Sophia Michel, LISW</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -3365,13 +3474,20 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="C13" t="s">
-        <v>93</v>
+        <v>89</v>
+      </c>
+      <c r="D13">
+        <v>6</v>
       </c>
       <c r="E13" t="s">
-        <v>94</v>
+        <v>90</v>
+      </c>
+      <c r="F13" t="str">
+        <f>C13 &amp; " " &amp; B13 &amp; ", " &amp; VLOOKUP($D13,Titles!$A$2:$B$11,2,FALSE)</f>
+        <v>Rhodie Shoesmith, D(ABMM)</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -3380,13 +3496,20 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="C14" t="s">
-        <v>96</v>
+        <v>92</v>
+      </c>
+      <c r="D14">
+        <v>7</v>
       </c>
       <c r="E14" t="s">
-        <v>97</v>
+        <v>93</v>
+      </c>
+      <c r="F14" t="str">
+        <f>C14 &amp; " " &amp; B14 &amp; ", " &amp; VLOOKUP($D14,Titles!$A$2:$B$11,2,FALSE)</f>
+        <v>Nonie Shields, DVM</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -3395,13 +3518,20 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="C15" t="s">
-        <v>99</v>
+        <v>95</v>
+      </c>
+      <c r="D15">
+        <v>8</v>
       </c>
       <c r="E15" t="s">
-        <v>100</v>
+        <v>96</v>
+      </c>
+      <c r="F15" t="str">
+        <f>C15 &amp; " " &amp; B15 &amp; ", " &amp; VLOOKUP($D15,Titles!$A$2:$B$11,2,FALSE)</f>
+        <v>Katina Tatlock, MD</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -3410,538 +3540,20 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C16" t="s">
-        <v>102</v>
+        <v>98</v>
+      </c>
+      <c r="D16">
+        <v>9</v>
       </c>
       <c r="E16" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <f t="shared" si="0"/>
-        <v>16</v>
-      </c>
-      <c r="B17" t="s">
-        <v>104</v>
-      </c>
-      <c r="C17" t="s">
-        <v>105</v>
-      </c>
-      <c r="E17" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <f t="shared" si="0"/>
-        <v>17</v>
-      </c>
-      <c r="B18" t="s">
-        <v>107</v>
-      </c>
-      <c r="C18" t="s">
-        <v>108</v>
-      </c>
-      <c r="E18" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <f t="shared" si="0"/>
-        <v>18</v>
-      </c>
-      <c r="B19" t="s">
-        <v>110</v>
-      </c>
-      <c r="C19" t="s">
-        <v>111</v>
-      </c>
-      <c r="E19" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <f t="shared" si="0"/>
-        <v>19</v>
-      </c>
-      <c r="B20" t="s">
-        <v>113</v>
-      </c>
-      <c r="C20" t="s">
-        <v>114</v>
-      </c>
-      <c r="E20" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="B21" t="s">
-        <v>116</v>
-      </c>
-      <c r="C21" t="s">
-        <v>117</v>
-      </c>
-      <c r="E21" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <f t="shared" si="0"/>
-        <v>21</v>
-      </c>
-      <c r="B22" t="s">
-        <v>119</v>
-      </c>
-      <c r="C22" t="s">
-        <v>120</v>
-      </c>
-      <c r="E22" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <f t="shared" si="0"/>
-        <v>22</v>
-      </c>
-      <c r="B23" t="s">
-        <v>122</v>
-      </c>
-      <c r="C23" t="s">
-        <v>123</v>
-      </c>
-      <c r="E23" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <f t="shared" si="0"/>
-        <v>23</v>
-      </c>
-      <c r="B24" t="s">
-        <v>125</v>
-      </c>
-      <c r="C24" t="s">
-        <v>126</v>
-      </c>
-      <c r="E24" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <f t="shared" si="0"/>
-        <v>24</v>
-      </c>
-      <c r="B25" t="s">
-        <v>128</v>
-      </c>
-      <c r="C25" t="s">
-        <v>129</v>
-      </c>
-      <c r="E25" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <f t="shared" si="0"/>
-        <v>25</v>
-      </c>
-      <c r="B26" t="s">
-        <v>131</v>
-      </c>
-      <c r="C26" t="s">
-        <v>132</v>
-      </c>
-      <c r="E26" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <f t="shared" si="0"/>
-        <v>26</v>
-      </c>
-      <c r="B27" t="s">
-        <v>134</v>
-      </c>
-      <c r="C27" t="s">
-        <v>135</v>
-      </c>
-      <c r="E27" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <f t="shared" si="0"/>
-        <v>27</v>
-      </c>
-      <c r="B28" t="s">
-        <v>137</v>
-      </c>
-      <c r="C28" t="s">
-        <v>138</v>
-      </c>
-      <c r="E28" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29">
-        <f t="shared" si="0"/>
-        <v>28</v>
-      </c>
-      <c r="B29" t="s">
-        <v>140</v>
-      </c>
-      <c r="C29" t="s">
-        <v>141</v>
-      </c>
-      <c r="E29" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30">
-        <f t="shared" si="0"/>
-        <v>29</v>
-      </c>
-      <c r="B30" t="s">
-        <v>143</v>
-      </c>
-      <c r="C30" t="s">
-        <v>144</v>
-      </c>
-      <c r="E30" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31">
-        <f t="shared" si="0"/>
-        <v>30</v>
-      </c>
-      <c r="B31" t="s">
-        <v>146</v>
-      </c>
-      <c r="C31" t="s">
-        <v>147</v>
-      </c>
-      <c r="E31" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32">
-        <f t="shared" si="0"/>
-        <v>31</v>
-      </c>
-      <c r="B32" t="s">
-        <v>149</v>
-      </c>
-      <c r="C32" t="s">
-        <v>150</v>
-      </c>
-      <c r="E32" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33">
-        <f t="shared" si="0"/>
-        <v>32</v>
-      </c>
-      <c r="B33" t="s">
-        <v>152</v>
-      </c>
-      <c r="C33" t="s">
-        <v>153</v>
-      </c>
-      <c r="E33" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34">
-        <f t="shared" si="0"/>
-        <v>33</v>
-      </c>
-      <c r="B34" t="s">
-        <v>155</v>
-      </c>
-      <c r="C34" t="s">
-        <v>156</v>
-      </c>
-      <c r="E34" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35">
-        <f t="shared" si="0"/>
-        <v>34</v>
-      </c>
-      <c r="B35" t="s">
-        <v>158</v>
-      </c>
-      <c r="C35" t="s">
-        <v>159</v>
-      </c>
-      <c r="E35" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36">
-        <f t="shared" si="0"/>
-        <v>35</v>
-      </c>
-      <c r="B36" t="s">
-        <v>161</v>
-      </c>
-      <c r="C36" t="s">
-        <v>162</v>
-      </c>
-      <c r="E36" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37">
-        <f t="shared" si="0"/>
-        <v>36</v>
-      </c>
-      <c r="B37" t="s">
-        <v>164</v>
-      </c>
-      <c r="C37" t="s">
-        <v>165</v>
-      </c>
-      <c r="E37" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38">
-        <f t="shared" si="0"/>
-        <v>37</v>
-      </c>
-      <c r="B38" t="s">
-        <v>167</v>
-      </c>
-      <c r="C38" t="s">
-        <v>168</v>
-      </c>
-      <c r="E38" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39">
-        <f t="shared" si="0"/>
-        <v>38</v>
-      </c>
-      <c r="B39" t="s">
-        <v>170</v>
-      </c>
-      <c r="C39" t="s">
-        <v>171</v>
-      </c>
-      <c r="E39" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40">
-        <f t="shared" si="0"/>
-        <v>39</v>
-      </c>
-      <c r="B40" t="s">
-        <v>173</v>
-      </c>
-      <c r="C40" t="s">
-        <v>174</v>
-      </c>
-      <c r="E40" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41">
-        <f t="shared" si="0"/>
-        <v>40</v>
-      </c>
-      <c r="B41" t="s">
-        <v>176</v>
-      </c>
-      <c r="C41" t="s">
-        <v>177</v>
-      </c>
-      <c r="E41" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42">
-        <f t="shared" si="0"/>
-        <v>41</v>
-      </c>
-      <c r="B42" t="s">
-        <v>179</v>
-      </c>
-      <c r="C42" t="s">
-        <v>180</v>
-      </c>
-      <c r="E42" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43">
-        <f t="shared" si="0"/>
-        <v>42</v>
-      </c>
-      <c r="B43" t="s">
-        <v>182</v>
-      </c>
-      <c r="C43" t="s">
-        <v>183</v>
-      </c>
-      <c r="E43" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44">
-        <f t="shared" si="0"/>
-        <v>43</v>
-      </c>
-      <c r="B44" t="s">
-        <v>185</v>
-      </c>
-      <c r="C44" t="s">
-        <v>186</v>
-      </c>
-      <c r="E44" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45">
-        <f t="shared" si="0"/>
-        <v>44</v>
-      </c>
-      <c r="B45" t="s">
-        <v>188</v>
-      </c>
-      <c r="C45" t="s">
-        <v>189</v>
-      </c>
-      <c r="E45" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46">
-        <f t="shared" si="0"/>
-        <v>45</v>
-      </c>
-      <c r="B46" t="s">
-        <v>191</v>
-      </c>
-      <c r="C46" t="s">
-        <v>192</v>
-      </c>
-      <c r="E46" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47">
-        <f t="shared" si="0"/>
-        <v>46</v>
-      </c>
-      <c r="B47" t="s">
-        <v>194</v>
-      </c>
-      <c r="C47" t="s">
-        <v>195</v>
-      </c>
-      <c r="E47" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48">
-        <f t="shared" si="0"/>
-        <v>47</v>
-      </c>
-      <c r="B48" t="s">
-        <v>197</v>
-      </c>
-      <c r="C48" t="s">
-        <v>198</v>
-      </c>
-      <c r="E48" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49">
-        <f t="shared" si="0"/>
-        <v>48</v>
-      </c>
-      <c r="B49" t="s">
-        <v>200</v>
-      </c>
-      <c r="C49" t="s">
-        <v>201</v>
-      </c>
-      <c r="E49" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50">
-        <f t="shared" si="0"/>
-        <v>49</v>
-      </c>
-      <c r="B50" t="s">
-        <v>203</v>
-      </c>
-      <c r="C50" t="s">
-        <v>204</v>
-      </c>
-      <c r="E50" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51">
-        <f t="shared" si="0"/>
-        <v>50</v>
-      </c>
-      <c r="B51" t="s">
-        <v>206</v>
-      </c>
-      <c r="C51" t="s">
-        <v>207</v>
-      </c>
-      <c r="E51" t="s">
-        <v>208</v>
+        <v>99</v>
+      </c>
+      <c r="F16" t="str">
+        <f>C16 &amp; " " &amp; B16 &amp; ", " &amp; VLOOKUP($D16,Titles!$A$2:$B$11,2,FALSE)</f>
+        <v>Don Ivan, MS</v>
       </c>
     </row>
   </sheetData>
@@ -3951,10 +3563,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B802DA53-C1DC-48A8-8ED8-C3684C54A4FB}">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3968,48 +3580,91 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
       <c r="B2" t="s">
-        <v>253</v>
+        <v>144</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <f>1+A2</f>
+        <v>2</v>
+      </c>
       <c r="B3" t="s">
-        <v>254</v>
+        <v>145</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <f t="shared" ref="A4:A10" si="0">1+A3</f>
+        <v>3</v>
+      </c>
       <c r="B4" t="s">
-        <v>255</v>
+        <v>146</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
       <c r="B5" t="s">
-        <v>256</v>
+        <v>147</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
       <c r="B6" t="s">
-        <v>257</v>
+        <v>148</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
       <c r="B7" t="s">
-        <v>258</v>
+        <v>149</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
       <c r="B8" t="s">
-        <v>259</v>
+        <v>150</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
       <c r="B9" t="s">
-        <v>253</v>
+        <v>144</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
       <c r="B10" t="s">
-        <v>260</v>
+        <v>151</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>152</v>
       </c>
     </row>
   </sheetData>
@@ -4018,40 +3673,6 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C46024E0-E270-4EA3-8E01-389F46224159}">
-  <dimension ref="A1:D1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C1" t="s">
-        <v>57</v>
-      </c>
-      <c r="D1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C41EDBA-D45F-4E05-8513-C5A89667080E}">
   <dimension ref="A1:B44"/>
   <sheetViews>

</xml_diff>